<commit_message>
migrate to new tables
</commit_message>
<xml_diff>
--- a/Projects/RBUS_SAND/Data/KPIs Template RB 180405.xlsx
+++ b/Projects/RBUS_SAND/Data/KPIs Template RB 180405.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
   <si>
     <t xml:space="preserve">KPI Level 1 Name</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">KPI description</t>
   </si>
   <si>
+    <t xml:space="preserve">Template for KPI</t>
+  </si>
+  <si>
     <t xml:space="preserve">Shelf occupation</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t xml:space="preserve">Number of Redbull shelves occupied</t>
   </si>
   <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
     <t xml:space="preserve">K002</t>
   </si>
   <si>
@@ -175,34 +181,49 @@
     <t xml:space="preserve">0041152875</t>
   </si>
   <si>
+    <t xml:space="preserve">Placement Count</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">placements</t>
+  </si>
+  <si>
     <t xml:space="preserve">placement count</t>
   </si>
   <si>
-    <t xml:space="preserve">K006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">placements</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of additional ambient placements in store</t>
   </si>
   <si>
+    <t xml:space="preserve">ADDITIONAL AMBIENT PLACEMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">K007</t>
   </si>
   <si>
     <t xml:space="preserve">Number of additional chilled placemetns in store</t>
   </si>
   <si>
+    <t xml:space="preserve">ADDITIONAL CHILLED PLACEMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">K008</t>
   </si>
   <si>
     <t xml:space="preserve">Number of additional chilled cashier cooler placements in store</t>
   </si>
   <si>
+    <t xml:space="preserve">CHILLED CASHIER PLACEMENT</t>
+  </si>
+  <si>
     <t xml:space="preserve">K009</t>
   </si>
   <si>
     <t xml:space="preserve">Number of additioanl chilled can coolers in store?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHILLED CAN COOLERS</t>
   </si>
 </sst>
 </file>
@@ -440,23 +461,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="28.7953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.246511627907"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="56.1162790697675"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.35348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.1209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.3953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="59.5627906976744"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="34.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -490,489 +512,543 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>14</v>
-      </c>
       <c r="I4" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="F6" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F9" s="6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F10" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F11" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F14" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>53</v>
-      </c>
       <c r="F16" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>58</v>
+        <v>63</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>